<commit_message>
New chart code and charts
</commit_message>
<xml_diff>
--- a/New IIASA Price data.xlsx
+++ b/New IIASA Price data.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="520" windowWidth="28560" windowHeight="17380"/>
+    <workbookView xWindow="240" yWindow="660" windowWidth="46360" windowHeight="25920"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$M$191</definedName>
+  </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -467,10 +470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -519,7 +523,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -560,7 +564,7 @@
         <v>385.34620000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -601,7 +605,7 @@
         <v>102.4367</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -642,7 +646,7 @@
         <v>38.962000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -683,7 +687,7 @@
         <v>940.68370000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -724,7 +728,7 @@
         <v>248.25129999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -765,7 +769,7 @@
         <v>117.0971</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -806,7 +810,7 @@
         <v>12.8607</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -847,7 +851,7 @@
         <v>1167.6774</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -888,7 +892,7 @@
         <v>446.91480000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
@@ -929,7 +933,7 @@
         <v>82.712900000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
@@ -970,7 +974,7 @@
         <v>296.12970000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1011,7 +1015,7 @@
         <v>64.061000000000007</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1052,7 +1056,7 @@
         <v>36.2684</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -1093,7 +1097,7 @@
         <v>1001.1420000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1134,7 +1138,7 @@
         <v>435.42430000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1179,7 @@
         <v>176.54169999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -1216,7 +1220,7 @@
         <v>54.079900000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1257,7 +1261,7 @@
         <v>784.49989090909105</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1298,7 +1302,7 @@
         <v>293.17560545454501</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1380,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>24</v>
       </c>
@@ -1421,7 +1425,7 @@
         <v>1853.2258363636399</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
@@ -1462,7 +1466,7 @@
         <v>815.873563636364</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1503,7 +1507,7 @@
         <v>317.78150727272703</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -1667,7 +1671,7 @@
         <v>2126.9061818181799</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
@@ -1708,7 +1712,7 @@
         <v>1053.1858909090899</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
@@ -1749,7 +1753,7 @@
         <v>201.06549818181799</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>24</v>
       </c>
@@ -1831,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>24</v>
       </c>
@@ -1872,7 +1876,7 @@
         <v>2254.1020363636399</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>24</v>
       </c>
@@ -1913,7 +1917,7 @@
         <v>1247.92396363636</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
@@ -1954,7 +1958,7 @@
         <v>361.77126545454502</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>24</v>
       </c>
@@ -2036,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
@@ -2077,7 +2081,7 @@
         <v>139.7414663151676</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
@@ -2200,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>31</v>
       </c>
@@ -2241,7 +2245,7 @@
         <v>748.57470777982473</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>31</v>
       </c>
@@ -2282,7 +2286,7 @@
         <v>314.6244676441699</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>31</v>
       </c>
@@ -2323,7 +2327,7 @@
         <v>101.88455210383768</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>31</v>
       </c>
@@ -2405,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>31</v>
       </c>
@@ -2446,7 +2450,7 @@
         <v>427.98925824048922</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>31</v>
       </c>
@@ -2487,7 +2491,7 @@
         <v>138.26629375065974</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>31</v>
       </c>
@@ -2569,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>32</v>
       </c>
@@ -2610,7 +2614,7 @@
         <v>508.49968000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>32</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>217.09107</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>32</v>
       </c>
@@ -2733,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>32</v>
       </c>
@@ -2774,7 +2778,7 @@
         <v>971.39858000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>32</v>
       </c>
@@ -2815,7 +2819,7 @@
         <v>346.83157</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>32</v>
       </c>
@@ -2856,7 +2860,7 @@
         <v>141.32957999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>32</v>
       </c>
@@ -2938,7 +2942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>32</v>
       </c>
@@ -2979,7 +2983,7 @@
         <v>1554.2899199999999</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -3020,7 +3024,7 @@
         <v>661.09082999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>32</v>
       </c>
@@ -3102,7 +3106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>33</v>
       </c>
@@ -3143,7 +3147,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>33</v>
       </c>
@@ -3184,7 +3188,7 @@
         <v>354.7</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>33</v>
       </c>
@@ -3266,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>33</v>
       </c>
@@ -3307,7 +3311,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>33</v>
       </c>
@@ -3348,7 +3352,7 @@
         <v>723.2</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>33</v>
       </c>
@@ -3389,7 +3393,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
@@ -3471,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>33</v>
       </c>
@@ -3512,7 +3516,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>33</v>
       </c>
@@ -3553,7 +3557,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>33</v>
       </c>
@@ -3594,7 +3598,7 @@
         <v>411.1</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>33</v>
       </c>
@@ -3676,7 +3680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>34</v>
       </c>
@@ -3717,7 +3721,7 @@
         <v>7098.5412610332769</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>34</v>
       </c>
@@ -3758,7 +3762,7 @@
         <v>1220.3433778459623</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>34</v>
       </c>
@@ -3840,7 +3844,7 @@
         <v>2.9089315732873375E-18</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>34</v>
       </c>
@@ -3881,7 +3885,7 @@
         <v>8320.6802163733228</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>34</v>
       </c>
@@ -3922,7 +3926,7 @@
         <v>1753.0805161923251</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>34</v>
       </c>
@@ -3963,7 +3967,7 @@
         <v>543.53782589158766</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>34</v>
       </c>
@@ -4004,7 +4008,7 @@
         <v>118.39024959966727</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>34</v>
       </c>
@@ -4045,7 +4049,7 @@
         <v>3230.9192479497938</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>34</v>
       </c>
@@ -4086,7 +4090,7 @@
         <v>625.03924163448085</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>34</v>
       </c>
@@ -4127,7 +4131,7 @@
         <v>115.7689189930426</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>34</v>
       </c>
@@ -4168,7 +4172,7 @@
         <v>3783.4027859301664</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>34</v>
       </c>
@@ -4209,7 +4213,7 @@
         <v>893.20014993202972</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>34</v>
       </c>
@@ -4291,7 +4295,7 @@
         <v>3.319344159890323E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>34</v>
       </c>
@@ -4332,7 +4336,7 @@
         <v>7861.386702732616</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>34</v>
       </c>
@@ -4373,7 +4377,7 @@
         <v>1634.0291851400657</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>34</v>
       </c>
@@ -4414,7 +4418,7 @@
         <v>426.01685658649279</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>4</v>
       </c>
@@ -4455,7 +4459,7 @@
         <v>385.34620000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>4</v>
       </c>
@@ -4496,7 +4500,7 @@
         <v>102.4367</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>4</v>
       </c>
@@ -4537,7 +4541,7 @@
         <v>38.962000000000003</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>4</v>
       </c>
@@ -4578,7 +4582,7 @@
         <v>940.68370000000004</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>4</v>
       </c>
@@ -4619,7 +4623,7 @@
         <v>248.25129999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>4</v>
       </c>
@@ -4660,7 +4664,7 @@
         <v>117.0971</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>4</v>
       </c>
@@ -4701,7 +4705,7 @@
         <v>12.8607</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>4</v>
       </c>
@@ -4742,7 +4746,7 @@
         <v>1167.6774</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>4</v>
       </c>
@@ -4783,7 +4787,7 @@
         <v>446.91480000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>4</v>
       </c>
@@ -4824,7 +4828,7 @@
         <v>82.712900000000005</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>4</v>
       </c>
@@ -4865,7 +4869,7 @@
         <v>296.12970000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>4</v>
       </c>
@@ -4906,7 +4910,7 @@
         <v>64.061000000000007</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>4</v>
       </c>
@@ -4947,7 +4951,7 @@
         <v>36.2684</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>4</v>
       </c>
@@ -4988,7 +4992,7 @@
         <v>1001.1420000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>4</v>
       </c>
@@ -5029,7 +5033,7 @@
         <v>435.42430000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>4</v>
       </c>
@@ -5070,7 +5074,7 @@
         <v>176.54169999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>4</v>
       </c>
@@ -5111,7 +5115,7 @@
         <v>54.079900000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>24</v>
       </c>
@@ -5152,7 +5156,7 @@
         <v>784.49989090909105</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>24</v>
       </c>
@@ -5193,7 +5197,7 @@
         <v>293.17560545454501</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>24</v>
       </c>
@@ -5275,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>24</v>
       </c>
@@ -5316,7 +5320,7 @@
         <v>1853.2258363636399</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>24</v>
       </c>
@@ -5357,7 +5361,7 @@
         <v>815.873563636364</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>24</v>
       </c>
@@ -5398,7 +5402,7 @@
         <v>317.78150727272703</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>24</v>
       </c>
@@ -5521,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>24</v>
       </c>
@@ -5562,7 +5566,7 @@
         <v>2126.9061818181799</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>24</v>
       </c>
@@ -5603,7 +5607,7 @@
         <v>1053.1858909090899</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>24</v>
       </c>
@@ -5644,7 +5648,7 @@
         <v>201.06549818181799</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>24</v>
       </c>
@@ -5726,7 +5730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>24</v>
       </c>
@@ -5767,7 +5771,7 @@
         <v>2254.1020363636399</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>24</v>
       </c>
@@ -5808,7 +5812,7 @@
         <v>1247.92396363636</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>24</v>
       </c>
@@ -5849,7 +5853,7 @@
         <v>361.77126545454502</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>24</v>
       </c>
@@ -5931,7 +5935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>31</v>
       </c>
@@ -5972,7 +5976,7 @@
         <v>139.7414663151676</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>31</v>
       </c>
@@ -6464,7 +6468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>32</v>
       </c>
@@ -6505,7 +6509,7 @@
         <v>508.49968000000001</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>32</v>
       </c>
@@ -6546,7 +6550,7 @@
         <v>217.09107</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>32</v>
       </c>
@@ -6628,7 +6632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>32</v>
       </c>
@@ -6669,7 +6673,7 @@
         <v>971.39858000000004</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>32</v>
       </c>
@@ -6710,7 +6714,7 @@
         <v>346.83157</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>32</v>
       </c>
@@ -6751,7 +6755,7 @@
         <v>141.32957999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>32</v>
       </c>
@@ -6833,7 +6837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>32</v>
       </c>
@@ -6874,7 +6878,7 @@
         <v>1554.2899199999999</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>32</v>
       </c>
@@ -6915,7 +6919,7 @@
         <v>661.09082999999998</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>32</v>
       </c>
@@ -6997,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>33</v>
       </c>
@@ -7038,7 +7042,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>33</v>
       </c>
@@ -7079,7 +7083,7 @@
         <v>354.7</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>33</v>
       </c>
@@ -7161,7 +7165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>33</v>
       </c>
@@ -7202,7 +7206,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>33</v>
       </c>
@@ -7243,7 +7247,7 @@
         <v>723.2</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>33</v>
       </c>
@@ -7284,7 +7288,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>33</v>
       </c>
@@ -7366,7 +7370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>33</v>
       </c>
@@ -7407,7 +7411,7 @@
         <v>3106</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>33</v>
       </c>
@@ -7448,7 +7452,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>33</v>
       </c>
@@ -7489,7 +7493,7 @@
         <v>411.1</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>33</v>
       </c>
@@ -7571,7 +7575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>34</v>
       </c>
@@ -7612,7 +7616,7 @@
         <v>7098.5412610332733</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>34</v>
       </c>
@@ -7653,7 +7657,7 @@
         <v>1220.3433778459626</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>34</v>
       </c>
@@ -7735,7 +7739,7 @@
         <v>2.9089315732873371E-18</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>34</v>
       </c>
@@ -7776,7 +7780,7 @@
         <v>8320.6802163733173</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>34</v>
       </c>
@@ -7817,7 +7821,7 @@
         <v>1753.0805161923247</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>34</v>
       </c>
@@ -7858,7 +7862,7 @@
         <v>543.53782589158766</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>34</v>
       </c>
@@ -7899,7 +7903,7 @@
         <v>118.39024959966729</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>34</v>
       </c>
@@ -7940,7 +7944,7 @@
         <v>3230.9192479497938</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>34</v>
       </c>
@@ -7981,7 +7985,7 @@
         <v>625.03924163448096</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>34</v>
       </c>
@@ -8022,7 +8026,7 @@
         <v>115.7689189930426</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>34</v>
       </c>
@@ -8063,7 +8067,7 @@
         <v>3783.40278593015</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>34</v>
       </c>
@@ -8104,7 +8108,7 @@
         <v>893.20014993202983</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>34</v>
       </c>
@@ -8186,7 +8190,7 @@
         <v>3.319344159890323E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>34</v>
       </c>
@@ -8227,7 +8231,7 @@
         <v>7861.386702732615</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>34</v>
       </c>
@@ -8268,7 +8272,7 @@
         <v>1634.0291851400657</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>34</v>
       </c>
@@ -8313,6 +8317,13 @@
       <c r="I196" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M191">
+    <filterColumn colId="5">
+      <customFilters>
+        <customFilter operator="lessThan" val="1"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>